<commit_message>
first correction SFN snippet
</commit_message>
<xml_diff>
--- a/Gayungan--002.xlsx
+++ b/Gayungan--002.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\DROPBOX\PA-DOC\CustomerHallo\TelKomSel--I\SKILLET\TSel--001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1F72C316-FB6C-48AA-827A-DCFE2C7C172C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FE67A04C-B726-4153-9529-090AB83487BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="90" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
+    <workbookView xWindow="135" yWindow="450" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
   <si>
     <t>ObjectTags</t>
   </si>
@@ -88,9 +88,6 @@
     <t>RAN-BLACK</t>
   </si>
   <si>
-    <t>{{ObjName}}</t>
-  </si>
-  <si>
     <t>SGSBY6-Gr-nic1</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>color38</t>
   </si>
   <si>
-    <t>{{ObjIPNetmask}}</t>
-  </si>
-  <si>
     <t>10.76.66.81/32</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Access Networks</t>
   </si>
   <si>
-    <t>{{ObjDescription}}</t>
-  </si>
-  <si>
     <t>VLAN 254 255</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>SFNForward</t>
   </si>
   <si>
-    <t>SFN_stamp.xml</t>
-  </si>
-  <si>
     <t>{{ SFN_SERVER }}</t>
   </si>
   <si>
@@ -275,6 +263,21 @@
   </si>
   <si>
     <t>/config/shared/log-settings</t>
+  </si>
+  <si>
+    <t>{{ ObjName }}</t>
+  </si>
+  <si>
+    <t>{{ TagName }}</t>
+  </si>
+  <si>
+    <t>{{ ObjDescription }}</t>
+  </si>
+  <si>
+    <t>{{ ObjIPNetmask }}</t>
+  </si>
+  <si>
+    <t>SFNSyslogServer_stamp.xml</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1144,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1173,11 +1176,11 @@
       </c>
       <c r="D1" s="60"/>
       <c r="E1" s="61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F1" s="62"/>
       <c r="G1" s="61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H1" s="62" t="s">
         <v>1</v>
@@ -1247,11 +1250,11 @@
       </c>
       <c r="D3" s="56"/>
       <c r="E3" s="55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" s="56"/>
       <c r="G3" s="55" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H3" s="56"/>
       <c r="I3" s="55"/>
@@ -1277,7 +1280,7 @@
       </c>
       <c r="F4" s="58"/>
       <c r="G4" s="57" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H4" s="58"/>
       <c r="I4" s="57"/>
@@ -1303,16 +1306,16 @@
         <v>13</v>
       </c>
       <c r="E6" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="65" t="s">
-        <v>15</v>
-      </c>
       <c r="G6" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
@@ -1327,16 +1330,16 @@
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="65" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>19</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -1353,16 +1356,16 @@
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="65" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="65" t="s">
-        <v>23</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
@@ -1381,10 +1384,10 @@
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
       <c r="E9" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -1404,7 +1407,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="67"/>
@@ -1423,16 +1426,16 @@
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F11" s="65" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -1449,16 +1452,16 @@
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F12" s="65" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
@@ -1477,10 +1480,10 @@
       <c r="C13" s="12"/>
       <c r="D13" s="16"/>
       <c r="E13" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F13" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="16"/>
@@ -1500,13 +1503,13 @@
         <v>12</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F14" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1523,10 +1526,10 @@
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E15" s="64"/>
       <c r="F15" s="65"/>
@@ -1545,16 +1548,16 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F16" s="65" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
@@ -1571,30 +1574,30 @@
       <c r="A17" s="10"/>
       <c r="B17" s="2"/>
       <c r="E17" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F17" s="65" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="2"/>
       <c r="E18" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F18" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="2"/>
       <c r="E19" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F19" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,40 +1610,40 @@
       <c r="A21" s="17"/>
       <c r="B21" s="2"/>
       <c r="E21" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F21" s="65" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="2"/>
       <c r="E22" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F22" s="65" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="2"/>
       <c r="E23" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F23" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="2"/>
       <c r="E24" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F24" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1653,30 +1656,30 @@
       <c r="A26" s="17"/>
       <c r="B26" s="2"/>
       <c r="E26" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="2"/>
       <c r="E27" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F27" s="65" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="2"/>
       <c r="E28" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,10 +1688,10 @@
       <c r="C29" s="18"/>
       <c r="D29" s="19"/>
       <c r="E29" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F29" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
@@ -1725,10 +1728,10 @@
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
       <c r="E31" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F31" s="65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
@@ -1747,10 +1750,10 @@
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
       <c r="E32" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F32" s="65" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
@@ -1769,10 +1772,10 @@
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
       <c r="E33" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F33" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="19"/>
@@ -1791,10 +1794,10 @@
       <c r="C34" s="18"/>
       <c r="D34" s="19"/>
       <c r="E34" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F34" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="19"/>
@@ -1831,10 +1834,10 @@
       <c r="C36" s="18"/>
       <c r="D36" s="19"/>
       <c r="E36" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F36" s="65" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="19"/>
@@ -1853,10 +1856,10 @@
       <c r="C37" s="18"/>
       <c r="D37" s="19"/>
       <c r="E37" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F37" s="65" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
@@ -1875,10 +1878,10 @@
       <c r="C38" s="18"/>
       <c r="D38" s="19"/>
       <c r="E38" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F38" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="19"/>
@@ -1897,10 +1900,10 @@
       <c r="C39" s="18"/>
       <c r="D39" s="19"/>
       <c r="E39" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F39" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="19"/>
@@ -1937,10 +1940,10 @@
       <c r="C41" s="18"/>
       <c r="D41" s="19"/>
       <c r="E41" s="64" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F41" s="65" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G41" s="18"/>
       <c r="H41" s="19"/>
@@ -1959,10 +1962,10 @@
       <c r="C42" s="18"/>
       <c r="D42" s="19"/>
       <c r="E42" s="64" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F42" s="65" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="19"/>
@@ -1981,10 +1984,10 @@
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
       <c r="E43" s="64" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F43" s="65" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="19"/>
@@ -2003,10 +2006,10 @@
       <c r="C44" s="18"/>
       <c r="D44" s="19"/>
       <c r="E44" s="64" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F44" s="65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="19"/>
@@ -2043,10 +2046,10 @@
       <c r="C46" s="18"/>
       <c r="D46" s="19"/>
       <c r="E46" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F46" s="69" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="19"/>
@@ -2065,10 +2068,10 @@
       <c r="C47" s="18"/>
       <c r="D47" s="19"/>
       <c r="E47" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F47" s="69" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="19"/>
@@ -2087,10 +2090,10 @@
       <c r="C48" s="18"/>
       <c r="D48" s="19"/>
       <c r="E48" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F48" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="19"/>
@@ -2109,10 +2112,10 @@
       <c r="C49" s="18"/>
       <c r="D49" s="19"/>
       <c r="E49" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F49" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G49" s="18"/>
       <c r="H49" s="19"/>
@@ -2149,10 +2152,10 @@
       <c r="C51" s="18"/>
       <c r="D51" s="19"/>
       <c r="E51" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F51" s="69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>
@@ -2171,10 +2174,10 @@
       <c r="C52" s="18"/>
       <c r="D52" s="19"/>
       <c r="E52" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F52" s="69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G52" s="18"/>
       <c r="H52" s="19"/>
@@ -2193,10 +2196,10 @@
       <c r="C53" s="20"/>
       <c r="D53" s="21"/>
       <c r="E53" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F53" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="21"/>
@@ -2214,10 +2217,10 @@
       <c r="B54" s="2"/>
       <c r="C54" s="18"/>
       <c r="E54" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F54" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G54" s="18"/>
       <c r="I54" s="18"/>
@@ -2249,10 +2252,10 @@
       <c r="C56" s="20"/>
       <c r="D56" s="21"/>
       <c r="E56" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F56" s="69" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
@@ -2271,10 +2274,10 @@
       <c r="C57" s="20"/>
       <c r="D57" s="24"/>
       <c r="E57" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F57" s="69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="24"/>
@@ -2293,10 +2296,10 @@
       <c r="C58" s="18"/>
       <c r="D58" s="26"/>
       <c r="E58" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F58" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="26"/>
@@ -2315,10 +2318,10 @@
       <c r="C59" s="18"/>
       <c r="D59" s="27"/>
       <c r="E59" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F59" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="27"/>
@@ -2355,10 +2358,10 @@
       <c r="C61" s="29"/>
       <c r="D61" s="30"/>
       <c r="E61" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F61" s="69" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="30"/>
@@ -2377,10 +2380,10 @@
       <c r="C62" s="29"/>
       <c r="D62" s="31"/>
       <c r="E62" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F62" s="69" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G62" s="29"/>
       <c r="H62" s="31"/>
@@ -2399,10 +2402,10 @@
       <c r="C63" s="29"/>
       <c r="D63" s="32"/>
       <c r="E63" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F63" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G63" s="29"/>
       <c r="H63" s="32"/>
@@ -2421,10 +2424,10 @@
       <c r="C64" s="18"/>
       <c r="D64" s="33"/>
       <c r="E64" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F64" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G64" s="18"/>
       <c r="H64" s="33"/>
@@ -2453,10 +2456,10 @@
       <c r="A66" s="17"/>
       <c r="B66" s="2"/>
       <c r="E66" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F66" s="69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2464,10 +2467,10 @@
       <c r="B67" s="2"/>
       <c r="D67" s="23"/>
       <c r="E67" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F67" s="69" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H67" s="23"/>
       <c r="J67" s="23"/>
@@ -2481,10 +2484,10 @@
       <c r="C68" s="18"/>
       <c r="D68" s="23"/>
       <c r="E68" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F68" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G68" s="18"/>
       <c r="H68" s="23"/>
@@ -2502,10 +2505,10 @@
       <c r="B69" s="2"/>
       <c r="D69" s="35"/>
       <c r="E69" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F69" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H69" s="35"/>
       <c r="J69" s="35"/>
@@ -2524,10 +2527,10 @@
       <c r="B71" s="2"/>
       <c r="D71" s="23"/>
       <c r="E71" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F71" s="69" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H71" s="23"/>
       <c r="J71" s="23"/>
@@ -2541,10 +2544,10 @@
       <c r="C72" s="18"/>
       <c r="D72" s="23"/>
       <c r="E72" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F72" s="69" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G72" s="18"/>
       <c r="H72" s="23"/>
@@ -2563,10 +2566,10 @@
       <c r="C73" s="18"/>
       <c r="D73" s="23"/>
       <c r="E73" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F73" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="23"/>
@@ -2584,10 +2587,10 @@
       <c r="B74" s="2"/>
       <c r="C74" s="18"/>
       <c r="E74" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F74" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G74" s="18"/>
       <c r="I74" s="18"/>
@@ -2619,10 +2622,10 @@
       <c r="C76" s="18"/>
       <c r="D76" s="23"/>
       <c r="E76" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F76" s="69" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G76" s="18"/>
       <c r="H76" s="23"/>
@@ -2641,10 +2644,10 @@
       <c r="C77" s="18"/>
       <c r="D77" s="23"/>
       <c r="E77" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F77" s="69" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="23"/>
@@ -2662,10 +2665,10 @@
       <c r="B78" s="2"/>
       <c r="C78" s="18"/>
       <c r="E78" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F78" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G78" s="18"/>
       <c r="I78" s="18"/>
@@ -2679,10 +2682,10 @@
       <c r="C79" s="18"/>
       <c r="D79" s="23"/>
       <c r="E79" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F79" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G79" s="18"/>
       <c r="H79" s="23"/>
@@ -2719,10 +2722,10 @@
       <c r="C81" s="18"/>
       <c r="D81" s="36"/>
       <c r="E81" s="68" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F81" s="69" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G81" s="18"/>
       <c r="H81" s="36"/>
@@ -2741,10 +2744,10 @@
       <c r="C82" s="18"/>
       <c r="D82" s="19"/>
       <c r="E82" s="68" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="F82" s="69" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G82" s="18"/>
       <c r="H82" s="19"/>
@@ -2763,10 +2766,10 @@
       <c r="C83" s="18"/>
       <c r="D83" s="36"/>
       <c r="E83" s="68" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="F83" s="69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G83" s="18"/>
       <c r="H83" s="36"/>
@@ -2785,10 +2788,10 @@
       <c r="C84" s="18"/>
       <c r="D84" s="36"/>
       <c r="E84" s="68" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F84" s="69" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G84" s="18"/>
       <c r="H84" s="36"/>
@@ -3982,26 +3985,26 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="51" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4010,26 +4013,26 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="51" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="51" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="53" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SFN Server Profile
</commit_message>
<xml_diff>
--- a/Gayungan--002.xlsx
+++ b/Gayungan--002.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\DROPBOX\PA-DOC\CustomerHallo\TelKomSel--I\SKILLET\TSel--001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FE67A04C-B726-4153-9529-090AB83487BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A78254-7CFD-4521-81A0-65CB6612C21B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="450" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
+    <workbookView xWindow="1080" yWindow="480" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
   <si>
     <t>ObjectTags</t>
   </si>
@@ -52,9 +52,6 @@
     <t>H-Colum</t>
   </si>
   <si>
-    <t>I-Colum</t>
-  </si>
-  <si>
     <t>K-Column</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
     <t>RAN-BLACK</t>
   </si>
   <si>
+    <t>{{ObjName}}</t>
+  </si>
+  <si>
     <t>SGSBY6-Gr-nic1</t>
   </si>
   <si>
@@ -97,6 +97,9 @@
     <t>color38</t>
   </si>
   <si>
+    <t>{{ObjIPNetmask}}</t>
+  </si>
+  <si>
     <t>10.76.66.81/32</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
     <t>Access Networks</t>
   </si>
   <si>
+    <t>{{ObjDescription}}</t>
+  </si>
+  <si>
     <t>VLAN 254 255</t>
   </si>
   <si>
@@ -256,28 +262,40 @@
     <t>SFNForward</t>
   </si>
   <si>
-    <t>{{ SFN_SERVER }}</t>
-  </si>
-  <si>
     <t>192.168.1.7</t>
   </si>
   <si>
-    <t>/config/shared/log-settings</t>
-  </si>
-  <si>
-    <t>{{ ObjName }}</t>
-  </si>
-  <si>
-    <t>{{ TagName }}</t>
-  </si>
-  <si>
-    <t>{{ ObjDescription }}</t>
-  </si>
-  <si>
-    <t>{{ ObjIPNetmask }}</t>
-  </si>
-  <si>
-    <t>SFNSyslogServer_stamp.xml</t>
+    <t>5514</t>
+  </si>
+  <si>
+    <t>5516</t>
+  </si>
+  <si>
+    <t>/config/shared/log-settings/syslog</t>
+  </si>
+  <si>
+    <t>{{ServerIP}}</t>
+  </si>
+  <si>
+    <t>{{Port}}</t>
+  </si>
+  <si>
+    <t>{{SFNStream}}</t>
+  </si>
+  <si>
+    <t>SFNSyslogSrv_stamp.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SFNSyslogProf_stamp.xml</t>
+  </si>
+  <si>
+    <t>/config/shared/log-settings/profiles</t>
+  </si>
+  <si>
+    <t>threat</t>
+  </si>
+  <si>
+    <t>gtp</t>
   </si>
 </sst>
 </file>
@@ -734,6 +752,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -755,56 +823,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1144,7 +1162,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1171,126 +1189,126 @@
     <row r="1" spans="1:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="61" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="68"/>
+      <c r="K1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="68"/>
+      <c r="M1" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="68"/>
+    </row>
+    <row r="2" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55"/>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="62"/>
-    </row>
-    <row r="2" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="C2" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="70"/>
+      <c r="E2" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="70"/>
+      <c r="G2" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="70"/>
+      <c r="I2" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="70"/>
+      <c r="K2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="55" t="s">
+      <c r="L2" s="70"/>
+      <c r="M2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="55" t="s">
+      <c r="N2" s="70"/>
+      <c r="O2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="55" t="s">
+      <c r="P2" s="70"/>
+    </row>
+    <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="55"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="56"/>
-    </row>
-    <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="56"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="70"/>
+      <c r="G3" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="70"/>
+      <c r="I3" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="70"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
     </row>
     <row r="4" spans="1:16" s="7" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="D4" s="72"/>
+      <c r="E4" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="58"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="72"/>
+      <c r="I4" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="72"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="72"/>
     </row>
     <row r="5" spans="1:16" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1300,25 +1318,29 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="57" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
+        <v>82</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
       <c r="M6" s="12"/>
@@ -1335,14 +1357,18 @@
       <c r="D7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="65" t="s">
+      <c r="E7" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
+      <c r="F7" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="15"/>
       <c r="K7" s="14"/>
@@ -1356,21 +1382,29 @@
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
+      <c r="E8" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
       <c r="M8" s="14"/>
@@ -1383,11 +1417,11 @@
       <c r="B9" s="11"/>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>21</v>
+      <c r="E9" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -1404,15 +1438,19 @@
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="I10" s="12"/>
       <c r="J10" s="15"/>
       <c r="K10" s="12"/>
@@ -1429,16 +1467,20 @@
         <v>15</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="65" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
       <c r="K11" s="14"/>
@@ -1452,19 +1494,23 @@
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="H12" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
       <c r="K12" s="14"/>
@@ -1479,11 +1525,11 @@
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="65" t="s">
-        <v>20</v>
+      <c r="E13" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>22</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="16"/>
@@ -1500,19 +1546,19 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="12"/>
       <c r="J14" s="15"/>
       <c r="K14" s="12"/>
@@ -1529,10 +1575,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
+        <v>29</v>
+      </c>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
       <c r="I15" s="14"/>
@@ -1548,19 +1594,19 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="65" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>31</v>
       </c>
       <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
       <c r="K16" s="14"/>
@@ -1573,113 +1619,113 @@
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="2"/>
-      <c r="E17" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="65" t="s">
-        <v>30</v>
+      <c r="E17" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="2"/>
-      <c r="E18" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="65" t="s">
-        <v>20</v>
+      <c r="E18" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="2"/>
-      <c r="E19" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="65" t="s">
-        <v>21</v>
+      <c r="E19" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="57" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="2"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="67"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="2"/>
-      <c r="E21" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="65" t="s">
-        <v>31</v>
+      <c r="E21" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="2"/>
-      <c r="E22" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="65" t="s">
-        <v>32</v>
+      <c r="E22" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="2"/>
-      <c r="E23" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="65" t="s">
-        <v>20</v>
+      <c r="E23" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="2"/>
-      <c r="E24" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="65" t="s">
-        <v>21</v>
+      <c r="E24" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="2"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="67"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="2"/>
-      <c r="E26" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="65" t="s">
-        <v>33</v>
+      <c r="E26" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="2"/>
-      <c r="E27" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="65" t="s">
-        <v>34</v>
+      <c r="E27" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="2"/>
-      <c r="E28" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="65" t="s">
-        <v>20</v>
+      <c r="E28" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,11 +1733,11 @@
       <c r="B29" s="2"/>
       <c r="C29" s="18"/>
       <c r="D29" s="19"/>
-      <c r="E29" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="65" t="s">
-        <v>21</v>
+      <c r="E29" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
@@ -1709,8 +1755,8 @@
       <c r="B30" s="2"/>
       <c r="C30" s="18"/>
       <c r="D30" s="19"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="67"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="18"/>
       <c r="H30" s="19"/>
       <c r="I30" s="18"/>
@@ -1727,11 +1773,11 @@
       <c r="B31" s="2"/>
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="65" t="s">
-        <v>35</v>
+      <c r="E31" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="57" t="s">
+        <v>37</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
@@ -1749,11 +1795,11 @@
       <c r="B32" s="2"/>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
-      <c r="E32" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="65" t="s">
-        <v>36</v>
+      <c r="E32" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="57" t="s">
+        <v>38</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
@@ -1771,11 +1817,11 @@
       <c r="B33" s="2"/>
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
-      <c r="E33" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="65" t="s">
-        <v>20</v>
+      <c r="E33" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="57" t="s">
+        <v>22</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="19"/>
@@ -1793,11 +1839,11 @@
       <c r="B34" s="2"/>
       <c r="C34" s="18"/>
       <c r="D34" s="19"/>
-      <c r="E34" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="65" t="s">
-        <v>21</v>
+      <c r="E34" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="19"/>
@@ -1815,8 +1861,8 @@
       <c r="B35" s="2"/>
       <c r="C35" s="18"/>
       <c r="D35" s="19"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="67"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="18"/>
       <c r="H35" s="19"/>
       <c r="I35" s="18"/>
@@ -1833,11 +1879,11 @@
       <c r="B36" s="2"/>
       <c r="C36" s="18"/>
       <c r="D36" s="19"/>
-      <c r="E36" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="65" t="s">
-        <v>37</v>
+      <c r="E36" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="57" t="s">
+        <v>39</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="19"/>
@@ -1855,11 +1901,11 @@
       <c r="B37" s="2"/>
       <c r="C37" s="18"/>
       <c r="D37" s="19"/>
-      <c r="E37" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="65" t="s">
-        <v>38</v>
+      <c r="E37" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="57" t="s">
+        <v>40</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
@@ -1877,11 +1923,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="18"/>
       <c r="D38" s="19"/>
-      <c r="E38" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="65" t="s">
-        <v>20</v>
+      <c r="E38" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="57" t="s">
+        <v>22</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="19"/>
@@ -1899,11 +1945,11 @@
       <c r="B39" s="2"/>
       <c r="C39" s="18"/>
       <c r="D39" s="19"/>
-      <c r="E39" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="65" t="s">
-        <v>21</v>
+      <c r="E39" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G39" s="18"/>
       <c r="H39" s="19"/>
@@ -1921,8 +1967,8 @@
       <c r="B40" s="2"/>
       <c r="C40" s="18"/>
       <c r="D40" s="19"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="67"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="59"/>
       <c r="G40" s="18"/>
       <c r="H40" s="19"/>
       <c r="I40" s="18"/>
@@ -1939,11 +1985,11 @@
       <c r="B41" s="2"/>
       <c r="C41" s="18"/>
       <c r="D41" s="19"/>
-      <c r="E41" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="65" t="s">
-        <v>39</v>
+      <c r="E41" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="57" t="s">
+        <v>41</v>
       </c>
       <c r="G41" s="18"/>
       <c r="H41" s="19"/>
@@ -1961,11 +2007,11 @@
       <c r="B42" s="2"/>
       <c r="C42" s="18"/>
       <c r="D42" s="19"/>
-      <c r="E42" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="65" t="s">
-        <v>40</v>
+      <c r="E42" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="57" t="s">
+        <v>42</v>
       </c>
       <c r="G42" s="18"/>
       <c r="H42" s="19"/>
@@ -1983,11 +2029,11 @@
       <c r="B43" s="2"/>
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="65" t="s">
-        <v>20</v>
+      <c r="E43" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="57" t="s">
+        <v>22</v>
       </c>
       <c r="G43" s="18"/>
       <c r="H43" s="19"/>
@@ -2005,11 +2051,11 @@
       <c r="B44" s="2"/>
       <c r="C44" s="18"/>
       <c r="D44" s="19"/>
-      <c r="E44" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" s="65" t="s">
-        <v>21</v>
+      <c r="E44" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="19"/>
@@ -2045,11 +2091,11 @@
       <c r="B46" s="2"/>
       <c r="C46" s="18"/>
       <c r="D46" s="19"/>
-      <c r="E46" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F46" s="69" t="s">
-        <v>50</v>
+      <c r="E46" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="61" t="s">
+        <v>52</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="19"/>
@@ -2067,11 +2113,11 @@
       <c r="B47" s="2"/>
       <c r="C47" s="18"/>
       <c r="D47" s="19"/>
-      <c r="E47" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F47" s="69" t="s">
-        <v>52</v>
+      <c r="E47" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="61" t="s">
+        <v>54</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="19"/>
@@ -2089,11 +2135,11 @@
       <c r="B48" s="2"/>
       <c r="C48" s="18"/>
       <c r="D48" s="19"/>
-      <c r="E48" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="69" t="s">
-        <v>51</v>
+      <c r="E48" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="19"/>
@@ -2111,11 +2157,11 @@
       <c r="B49" s="2"/>
       <c r="C49" s="18"/>
       <c r="D49" s="19"/>
-      <c r="E49" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F49" s="69" t="s">
-        <v>26</v>
+      <c r="E49" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G49" s="18"/>
       <c r="H49" s="19"/>
@@ -2133,8 +2179,8 @@
       <c r="B50" s="2"/>
       <c r="C50" s="18"/>
       <c r="D50" s="19"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="71"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="63"/>
       <c r="G50" s="18"/>
       <c r="H50" s="19"/>
       <c r="I50" s="18"/>
@@ -2151,11 +2197,11 @@
       <c r="B51" s="2"/>
       <c r="C51" s="18"/>
       <c r="D51" s="19"/>
-      <c r="E51" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F51" s="69" t="s">
-        <v>66</v>
+      <c r="E51" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="61" t="s">
+        <v>68</v>
       </c>
       <c r="G51" s="18"/>
       <c r="H51" s="19"/>
@@ -2173,11 +2219,11 @@
       <c r="B52" s="2"/>
       <c r="C52" s="18"/>
       <c r="D52" s="19"/>
-      <c r="E52" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F52" s="69" t="s">
-        <v>65</v>
+      <c r="E52" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="61" t="s">
+        <v>67</v>
       </c>
       <c r="G52" s="18"/>
       <c r="H52" s="19"/>
@@ -2195,11 +2241,11 @@
       <c r="B53" s="2"/>
       <c r="C53" s="20"/>
       <c r="D53" s="21"/>
-      <c r="E53" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F53" s="69" t="s">
-        <v>51</v>
+      <c r="E53" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G53" s="20"/>
       <c r="H53" s="21"/>
@@ -2216,11 +2262,11 @@
       <c r="A54" s="22"/>
       <c r="B54" s="2"/>
       <c r="C54" s="18"/>
-      <c r="E54" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F54" s="69" t="s">
-        <v>26</v>
+      <c r="E54" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G54" s="18"/>
       <c r="I54" s="18"/>
@@ -2233,8 +2279,8 @@
       <c r="B55" s="2"/>
       <c r="C55" s="18"/>
       <c r="D55" s="23"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="72"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="64"/>
       <c r="G55" s="18"/>
       <c r="H55" s="23"/>
       <c r="I55" s="18"/>
@@ -2251,11 +2297,11 @@
       <c r="B56" s="2"/>
       <c r="C56" s="20"/>
       <c r="D56" s="21"/>
-      <c r="E56" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" s="69" t="s">
-        <v>63</v>
+      <c r="E56" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="61" t="s">
+        <v>65</v>
       </c>
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
@@ -2273,11 +2319,11 @@
       <c r="B57" s="2"/>
       <c r="C57" s="20"/>
       <c r="D57" s="24"/>
-      <c r="E57" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F57" s="69" t="s">
-        <v>64</v>
+      <c r="E57" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="61" t="s">
+        <v>66</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="24"/>
@@ -2295,11 +2341,11 @@
       <c r="B58" s="2"/>
       <c r="C58" s="18"/>
       <c r="D58" s="26"/>
-      <c r="E58" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F58" s="69" t="s">
-        <v>51</v>
+      <c r="E58" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G58" s="18"/>
       <c r="H58" s="26"/>
@@ -2317,11 +2363,11 @@
       <c r="B59" s="2"/>
       <c r="C59" s="18"/>
       <c r="D59" s="27"/>
-      <c r="E59" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F59" s="69" t="s">
-        <v>26</v>
+      <c r="E59" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G59" s="18"/>
       <c r="H59" s="27"/>
@@ -2339,8 +2385,8 @@
       <c r="B60" s="2"/>
       <c r="C60" s="18"/>
       <c r="D60" s="26"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="73"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="65"/>
       <c r="G60" s="18"/>
       <c r="H60" s="26"/>
       <c r="I60" s="18"/>
@@ -2357,11 +2403,11 @@
       <c r="B61" s="28"/>
       <c r="C61" s="29"/>
       <c r="D61" s="30"/>
-      <c r="E61" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F61" s="69" t="s">
-        <v>61</v>
+      <c r="E61" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="61" t="s">
+        <v>63</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="30"/>
@@ -2379,11 +2425,11 @@
       <c r="B62" s="28"/>
       <c r="C62" s="29"/>
       <c r="D62" s="31"/>
-      <c r="E62" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F62" s="69" t="s">
-        <v>62</v>
+      <c r="E62" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="61" t="s">
+        <v>64</v>
       </c>
       <c r="G62" s="29"/>
       <c r="H62" s="31"/>
@@ -2401,11 +2447,11 @@
       <c r="B63" s="28"/>
       <c r="C63" s="29"/>
       <c r="D63" s="32"/>
-      <c r="E63" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F63" s="69" t="s">
-        <v>51</v>
+      <c r="E63" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G63" s="29"/>
       <c r="H63" s="32"/>
@@ -2423,11 +2469,11 @@
       <c r="B64" s="28"/>
       <c r="C64" s="18"/>
       <c r="D64" s="33"/>
-      <c r="E64" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" s="69" t="s">
-        <v>26</v>
+      <c r="E64" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G64" s="18"/>
       <c r="H64" s="33"/>
@@ -2444,8 +2490,8 @@
       <c r="A65" s="17"/>
       <c r="B65" s="2"/>
       <c r="D65" s="34"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="74"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="66"/>
       <c r="H65" s="34"/>
       <c r="J65" s="34"/>
       <c r="L65" s="34"/>
@@ -2455,22 +2501,22 @@
     <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17"/>
       <c r="B66" s="2"/>
-      <c r="E66" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F66" s="69" t="s">
-        <v>59</v>
+      <c r="E66" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="61" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="2"/>
       <c r="D67" s="23"/>
-      <c r="E67" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F67" s="69" t="s">
-        <v>60</v>
+      <c r="E67" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="61" t="s">
+        <v>62</v>
       </c>
       <c r="H67" s="23"/>
       <c r="J67" s="23"/>
@@ -2483,11 +2529,11 @@
       <c r="B68" s="2"/>
       <c r="C68" s="18"/>
       <c r="D68" s="23"/>
-      <c r="E68" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F68" s="69" t="s">
-        <v>51</v>
+      <c r="E68" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G68" s="18"/>
       <c r="H68" s="23"/>
@@ -2504,11 +2550,11 @@
       <c r="A69" s="17"/>
       <c r="B69" s="2"/>
       <c r="D69" s="35"/>
-      <c r="E69" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F69" s="69" t="s">
-        <v>26</v>
+      <c r="E69" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="H69" s="35"/>
       <c r="J69" s="35"/>
@@ -2519,18 +2565,18 @@
     <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17"/>
       <c r="B70" s="2"/>
-      <c r="E70" s="70"/>
-      <c r="F70" s="71"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="63"/>
     </row>
     <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17"/>
       <c r="B71" s="2"/>
       <c r="D71" s="23"/>
-      <c r="E71" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F71" s="69" t="s">
-        <v>57</v>
+      <c r="E71" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="61" t="s">
+        <v>59</v>
       </c>
       <c r="H71" s="23"/>
       <c r="J71" s="23"/>
@@ -2543,11 +2589,11 @@
       <c r="B72" s="2"/>
       <c r="C72" s="18"/>
       <c r="D72" s="23"/>
-      <c r="E72" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F72" s="69" t="s">
-        <v>58</v>
+      <c r="E72" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="61" t="s">
+        <v>60</v>
       </c>
       <c r="G72" s="18"/>
       <c r="H72" s="23"/>
@@ -2565,11 +2611,11 @@
       <c r="B73" s="2"/>
       <c r="C73" s="18"/>
       <c r="D73" s="23"/>
-      <c r="E73" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F73" s="69" t="s">
-        <v>51</v>
+      <c r="E73" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F73" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="23"/>
@@ -2586,11 +2632,11 @@
       <c r="A74" s="17"/>
       <c r="B74" s="2"/>
       <c r="C74" s="18"/>
-      <c r="E74" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F74" s="69" t="s">
-        <v>26</v>
+      <c r="E74" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G74" s="18"/>
       <c r="I74" s="18"/>
@@ -2603,8 +2649,8 @@
       <c r="B75" s="2"/>
       <c r="C75" s="18"/>
       <c r="D75" s="23"/>
-      <c r="E75" s="70"/>
-      <c r="F75" s="72"/>
+      <c r="E75" s="62"/>
+      <c r="F75" s="64"/>
       <c r="G75" s="18"/>
       <c r="H75" s="23"/>
       <c r="I75" s="18"/>
@@ -2621,11 +2667,11 @@
       <c r="B76" s="2"/>
       <c r="C76" s="18"/>
       <c r="D76" s="23"/>
-      <c r="E76" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F76" s="69" t="s">
-        <v>55</v>
+      <c r="E76" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="61" t="s">
+        <v>57</v>
       </c>
       <c r="G76" s="18"/>
       <c r="H76" s="23"/>
@@ -2643,11 +2689,11 @@
       <c r="B77" s="2"/>
       <c r="C77" s="18"/>
       <c r="D77" s="23"/>
-      <c r="E77" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F77" s="69" t="s">
-        <v>56</v>
+      <c r="E77" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F77" s="61" t="s">
+        <v>58</v>
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="23"/>
@@ -2664,11 +2710,11 @@
       <c r="A78" s="17"/>
       <c r="B78" s="2"/>
       <c r="C78" s="18"/>
-      <c r="E78" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F78" s="69" t="s">
-        <v>51</v>
+      <c r="E78" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G78" s="18"/>
       <c r="I78" s="18"/>
@@ -2681,11 +2727,11 @@
       <c r="B79" s="2"/>
       <c r="C79" s="18"/>
       <c r="D79" s="23"/>
-      <c r="E79" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F79" s="69" t="s">
-        <v>26</v>
+      <c r="E79" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G79" s="18"/>
       <c r="H79" s="23"/>
@@ -2703,8 +2749,8 @@
       <c r="B80" s="2"/>
       <c r="C80" s="18"/>
       <c r="D80" s="23"/>
-      <c r="E80" s="70"/>
-      <c r="F80" s="72"/>
+      <c r="E80" s="62"/>
+      <c r="F80" s="64"/>
       <c r="G80" s="18"/>
       <c r="H80" s="23"/>
       <c r="I80" s="18"/>
@@ -2721,11 +2767,11 @@
       <c r="B81" s="2"/>
       <c r="C81" s="18"/>
       <c r="D81" s="36"/>
-      <c r="E81" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F81" s="69" t="s">
-        <v>54</v>
+      <c r="E81" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="61" t="s">
+        <v>56</v>
       </c>
       <c r="G81" s="18"/>
       <c r="H81" s="36"/>
@@ -2743,11 +2789,11 @@
       <c r="B82" s="2"/>
       <c r="C82" s="18"/>
       <c r="D82" s="19"/>
-      <c r="E82" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="F82" s="69" t="s">
-        <v>53</v>
+      <c r="E82" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F82" s="61" t="s">
+        <v>55</v>
       </c>
       <c r="G82" s="18"/>
       <c r="H82" s="19"/>
@@ -2765,11 +2811,11 @@
       <c r="B83" s="2"/>
       <c r="C83" s="18"/>
       <c r="D83" s="36"/>
-      <c r="E83" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="F83" s="69" t="s">
-        <v>51</v>
+      <c r="E83" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="G83" s="18"/>
       <c r="H83" s="36"/>
@@ -2787,11 +2833,11 @@
       <c r="B84" s="2"/>
       <c r="C84" s="18"/>
       <c r="D84" s="36"/>
-      <c r="E84" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F84" s="69" t="s">
-        <v>26</v>
+      <c r="E84" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="61" t="s">
+        <v>28</v>
       </c>
       <c r="G84" s="18"/>
       <c r="H84" s="36"/>
@@ -3920,6 +3966,26 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="28">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="M3:N3"/>
@@ -3928,35 +3994,7 @@
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3" xr:uid="{8C658EFA-4448-4BD7-A05C-A2EAE6B9E331}">
-      <formula1>yesno</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:P2" xr:uid="{F4172593-C9A0-48D4-87A4-4EECCA8767CE}">
-      <formula1>ynl</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="144" verticalDpi="144" r:id="rId1"/>
 </worksheet>
@@ -3970,7 +4008,7 @@
   <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3985,26 +4023,26 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="51" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4013,26 +4051,26 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="51" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="53" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing SFN new vars
</commit_message>
<xml_diff>
--- a/Gayungan--002.xlsx
+++ b/Gayungan--002.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\DROPBOX\PA-DOC\CustomerHallo\TelKomSel--I\SKILLET\TSel--001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A78254-7CFD-4521-81A0-65CB6612C21B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190A400-4D2C-423C-9E8E-C4DAA4F26A9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="480" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
+    <workbookView xWindow="570" yWindow="540" windowWidth="21540" windowHeight="12465" activeTab="1" xr2:uid="{276797BC-6ABC-4CB3-B4A9-E304FA023B27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -274,15 +274,6 @@
     <t>/config/shared/log-settings/syslog</t>
   </si>
   <si>
-    <t>{{ServerIP}}</t>
-  </si>
-  <si>
-    <t>{{Port}}</t>
-  </si>
-  <si>
-    <t>{{SFNStream}}</t>
-  </si>
-  <si>
     <t>SFNSyslogSrv_stamp.xml</t>
   </si>
   <si>
@@ -296,6 +287,15 @@
   </si>
   <si>
     <t>gtp</t>
+  </si>
+  <si>
+    <t>{{FWLogStream}}</t>
+  </si>
+  <si>
+    <t>{{SFNPort}}</t>
+  </si>
+  <si>
+    <t>{{SFNServerIP}}</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1268,11 +1268,11 @@
       </c>
       <c r="F3" s="70"/>
       <c r="G3" s="69" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H3" s="70"/>
       <c r="I3" s="69" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" s="70"/>
       <c r="K3" s="69"/>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="H4" s="72"/>
       <c r="I4" s="71" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J4" s="72"/>
       <c r="K4" s="71"/>
@@ -1330,16 +1330,16 @@
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
@@ -1364,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>73</v>
@@ -1394,16 +1394,16 @@
         <v>22</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>72</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -1446,10 +1446,10 @@
       <c r="E10" s="58"/>
       <c r="F10" s="59"/>
       <c r="G10" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="15"/>
@@ -1476,7 +1476,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>74</v>
@@ -1506,7 +1506,7 @@
         <v>27</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>72</v>
@@ -4008,7 +4008,7 @@
   <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>